<commit_message>
adjust params to lower gain=1 current to keep shape up to gain=2
</commit_message>
<xml_diff>
--- a/amp/amp.xlsx
+++ b/amp/amp.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjk/projects/synthesizer/amp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{858B1EF8-F557-3441-A77D-B03BCB5FAF24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3816991A-8C8B-2740-A148-4E200631E7EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{6400FE91-138F-4D41-B9CE-9D9E08F46C3F}"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="28040" windowHeight="17540" xr2:uid="{6400FE91-138F-4D41-B9CE-9D9E08F46C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>VB/26mV</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>IOUT (mA)</t>
+  </si>
+  <si>
+    <t>Iref (mA)</t>
+  </si>
+  <si>
+    <t>Imax (mA)</t>
+  </si>
+  <si>
+    <t>Rref (kohm)</t>
   </si>
 </sst>
 </file>
@@ -420,28 +429,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541F8547-BF2A-374F-80CA-51B3B3BC1C08}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,37 +462,46 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-6</v>
       </c>
@@ -488,46 +510,56 @@
         <v>403.42879349273511</v>
       </c>
       <c r="C2">
-        <f>MIN(2,B2)</f>
         <v>2</v>
       </c>
       <c r="D2">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <f>MIN(C2,B2*D2)</f>
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <f>12/D2</f>
+        <v>24</v>
+      </c>
+      <c r="G2">
         <f>A2*0.026</f>
         <v>-0.156</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <f>-(3.3/120)</f>
         <v>-2.75E-2</v>
       </c>
-      <c r="F2">
-        <f>D2/E2</f>
+      <c r="I2">
+        <f>G2/H2</f>
         <v>5.6727272727272728</v>
       </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <f>F2+G2</f>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <f>I2+J2</f>
         <v>10.672727272727272</v>
       </c>
-      <c r="I2">
-        <f>0.5*(20/26)*C2</f>
+      <c r="L2">
+        <f>0.5*(20/26)*E2</f>
         <v>0.76923076923076927</v>
       </c>
-      <c r="J2">
-        <f>5/I$8</f>
-        <v>13</v>
-      </c>
-      <c r="K2">
-        <f>(I2*J2)/5</f>
-        <v>2</v>
-      </c>
-      <c r="L2">
-        <f>20*LOG10(K2)</f>
-        <v>6.0205999132796242</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <f>5/L$8</f>
+        <v>26</v>
+      </c>
+      <c r="N2">
+        <f>(L2*M2)/5</f>
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <f>20*LOG10(N2)</f>
+        <v>12.041199826559248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-5</v>
       </c>
@@ -536,46 +568,56 @@
         <v>148.4131591025766</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C14" si="1">MIN(2,B3)</f>
         <v>2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D14" si="2">A3*0.026</f>
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E14" si="1">MIN(C3,B3*D3)</f>
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F14" si="2">12/D3</f>
+        <v>24</v>
+      </c>
+      <c r="G3">
+        <f>A3*0.026</f>
         <v>-0.13</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E14" si="3">-(3.3/120)</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H14" si="3">-(3.3/120)</f>
         <v>-2.75E-2</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F14" si="4">D3/E3</f>
+      <c r="I3">
+        <f t="shared" ref="I3:I14" si="4">G3/H3</f>
         <v>4.7272727272727275</v>
       </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H14" si="5">F3+G3</f>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K14" si="5">I3+J3</f>
         <v>9.7272727272727266</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I14" si="6">0.5*(20/26)*C3</f>
+      <c r="L3">
+        <f t="shared" ref="L3:L14" si="6">0.5*(20/26)*E3</f>
         <v>0.76923076923076927</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J14" si="7">5/I$8</f>
-        <v>13</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K14" si="8">(I3*J3)/5</f>
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L14" si="9">20*LOG10(K3)</f>
-        <v>6.0205999132796242</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <f t="shared" ref="M3:M14" si="7">5/L$8</f>
+        <v>26</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N14" si="8">(L3*M3)/5</f>
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O14" si="9">20*LOG10(N3)</f>
+        <v>12.041199826559248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-4</v>
       </c>
@@ -584,46 +626,56 @@
         <v>54.598150033144236</v>
       </c>
       <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <f>A4*0.026</f>
         <v>-0.104</v>
       </c>
-      <c r="E4">
+      <c r="H4">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <f t="shared" si="4"/>
         <v>3.7818181818181817</v>
       </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
         <f t="shared" si="5"/>
         <v>8.7818181818181813</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <f t="shared" si="6"/>
         <v>0.76923076923076927</v>
       </c>
-      <c r="J4">
+      <c r="M4">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K4">
+        <v>26</v>
+      </c>
+      <c r="N4">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="O4">
         <f t="shared" si="9"/>
-        <v>6.0205999132796242</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>12.041199826559248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-3</v>
       </c>
@@ -632,46 +684,56 @@
         <v>20.085536923187668</v>
       </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <f>A5*0.026</f>
         <v>-7.8E-2</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <f t="shared" si="4"/>
         <v>2.8363636363636364</v>
       </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="5"/>
         <v>7.836363636363636</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <f t="shared" si="6"/>
         <v>0.76923076923076927</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K5">
+        <v>26</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="9"/>
-        <v>6.0205999132796242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>12.041199826559248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-2</v>
       </c>
@@ -680,46 +742,56 @@
         <v>7.3890560989306504</v>
       </c>
       <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <f>A6*0.026</f>
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="E6">
+      <c r="H6">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <f t="shared" si="4"/>
         <v>1.8909090909090909</v>
       </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6">
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="5"/>
         <v>6.8909090909090907</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <f t="shared" si="6"/>
         <v>0.76923076923076927</v>
       </c>
-      <c r="J6">
+      <c r="M6">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K6">
+        <v>26</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="9"/>
-        <v>6.0205999132796242</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>12.041199826559248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-1</v>
       </c>
@@ -728,46 +800,56 @@
         <v>2.7182818284590451</v>
       </c>
       <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D7">
+        <v>1.3591409142295225</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G7">
+        <f>A7*0.026</f>
         <v>-2.5999999999999999E-2</v>
       </c>
-      <c r="E7">
+      <c r="H7">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <f t="shared" si="4"/>
         <v>0.94545454545454544</v>
       </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="5"/>
         <v>5.9454545454545453</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <f t="shared" si="6"/>
-        <v>0.76923076923076927</v>
-      </c>
-      <c r="J7">
+        <v>0.52274650547289336</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K7">
+        <v>26</v>
+      </c>
+      <c r="N7">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="L7">
+        <v>2.7182818284590455</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="9"/>
-        <v>6.0205999132796242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>8.6858896380650368</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -776,46 +858,56 @@
         <v>1</v>
       </c>
       <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <f>A8*0.026</f>
         <v>0</v>
       </c>
-      <c r="E8">
+      <c r="H8">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F8">
+      <c r="I8">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8">
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <f t="shared" si="6"/>
-        <v>0.38461538461538464</v>
-      </c>
-      <c r="J8">
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K8">
+        <v>26</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="L8">
+      <c r="O8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -824,46 +916,56 @@
         <v>0.36787944117144233</v>
       </c>
       <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="1"/>
-        <v>0.36787944117144233</v>
-      </c>
-      <c r="D9">
+        <v>0.18393972058572117</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <f>A9*0.026</f>
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="E9">
+      <c r="H9">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F9">
+      <c r="I9">
         <f t="shared" si="4"/>
         <v>-0.94545454545454544</v>
       </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-      <c r="H9">
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="5"/>
         <v>4.0545454545454547</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <f t="shared" si="6"/>
-        <v>0.14149209275824706</v>
-      </c>
-      <c r="J9">
+        <v>7.0746046379123531E-2</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K9">
+        <v>26</v>
+      </c>
+      <c r="N9">
         <f t="shared" si="8"/>
         <v>0.36787944117144239</v>
       </c>
-      <c r="L9">
+      <c r="O9">
         <f t="shared" si="9"/>
         <v>-8.685889638065035</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -872,46 +974,56 @@
         <v>0.1353352832366127</v>
       </c>
       <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="1"/>
-        <v>0.1353352832366127</v>
-      </c>
-      <c r="D10">
+        <v>6.7667641618306351E-2</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G10">
+        <f>A10*0.026</f>
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="E10">
+      <c r="H10">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F10">
+      <c r="I10">
         <f t="shared" si="4"/>
         <v>-1.8909090909090909</v>
       </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10">
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="5"/>
         <v>3.1090909090909093</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <f t="shared" si="6"/>
-        <v>5.205203201408181E-2</v>
-      </c>
-      <c r="J10">
+        <v>2.6026016007040905E-2</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K10">
+        <v>26</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="8"/>
         <v>0.1353352832366127</v>
       </c>
-      <c r="L10">
+      <c r="O10">
         <f t="shared" si="9"/>
         <v>-17.371779276130074</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -920,46 +1032,56 @@
         <v>4.9787068367863944E-2</v>
       </c>
       <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="1"/>
-        <v>4.9787068367863944E-2</v>
-      </c>
-      <c r="D11">
+        <v>2.4893534183931972E-2</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <f>A11*0.026</f>
         <v>7.8E-2</v>
       </c>
-      <c r="E11">
+      <c r="H11">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F11">
+      <c r="I11">
         <f t="shared" si="4"/>
         <v>-2.8363636363636364</v>
       </c>
-      <c r="G11">
-        <v>5</v>
-      </c>
-      <c r="H11">
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
         <f t="shared" si="5"/>
         <v>2.1636363636363636</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <f t="shared" si="6"/>
-        <v>1.9148872449178442E-2</v>
-      </c>
-      <c r="J11">
+        <v>9.5744362245892209E-3</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K11">
+        <v>26</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="8"/>
         <v>4.9787068367863951E-2</v>
       </c>
-      <c r="L11">
+      <c r="O11">
         <f t="shared" si="9"/>
         <v>-26.057668914195105</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -968,46 +1090,56 @@
         <v>1.8315638888734179E-2</v>
       </c>
       <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="1"/>
-        <v>1.8315638888734179E-2</v>
-      </c>
-      <c r="D12">
+        <v>9.1578194443670893E-3</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G12">
+        <f>A12*0.026</f>
         <v>0.104</v>
       </c>
-      <c r="E12">
+      <c r="H12">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F12">
+      <c r="I12">
         <f t="shared" si="4"/>
         <v>-3.7818181818181817</v>
       </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12">
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="5"/>
         <v>1.2181818181818183</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <f t="shared" si="6"/>
-        <v>7.0444764956669919E-3</v>
-      </c>
-      <c r="J12">
+        <v>3.5222382478334959E-3</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K12">
+        <v>26</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="8"/>
         <v>1.8315638888734179E-2</v>
       </c>
-      <c r="L12">
+      <c r="O12">
         <f t="shared" si="9"/>
         <v>-34.743558552260147</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1016,46 +1148,56 @@
         <v>6.737946999085467E-3</v>
       </c>
       <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="1"/>
-        <v>6.737946999085467E-3</v>
-      </c>
-      <c r="D13">
+        <v>3.3689734995427335E-3</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G13">
+        <f>A13*0.026</f>
         <v>0.13</v>
       </c>
-      <c r="E13">
+      <c r="H13">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F13">
+      <c r="I13">
         <f t="shared" si="4"/>
         <v>-4.7272727272727275</v>
       </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13">
+      <c r="J13">
+        <v>5</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="5"/>
         <v>0.27272727272727249</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <f t="shared" si="6"/>
-        <v>2.5915180765713336E-3</v>
-      </c>
-      <c r="J13">
+        <v>1.2957590382856668E-3</v>
+      </c>
+      <c r="M13">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K13">
+        <v>26</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="8"/>
         <v>6.737946999085467E-3</v>
       </c>
-      <c r="L13">
+      <c r="O13">
         <f t="shared" si="9"/>
         <v>-43.429448190325182</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1064,41 +1206,51 @@
         <v>2.4787521766663585E-3</v>
       </c>
       <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="1"/>
-        <v>2.4787521766663585E-3</v>
-      </c>
-      <c r="D14">
+        <v>1.2393760883331792E-3</v>
+      </c>
+      <c r="F14">
         <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="G14">
+        <f>A14*0.026</f>
         <v>0.156</v>
       </c>
-      <c r="E14">
+      <c r="H14">
         <f t="shared" si="3"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="F14">
+      <c r="I14">
         <f t="shared" si="4"/>
         <v>-5.6727272727272728</v>
       </c>
-      <c r="G14">
-        <v>5</v>
-      </c>
-      <c r="H14">
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="5"/>
         <v>-0.67272727272727284</v>
       </c>
-      <c r="I14">
+      <c r="L14">
         <f t="shared" si="6"/>
-        <v>9.5336622179475333E-4</v>
-      </c>
-      <c r="J14">
+        <v>4.7668311089737667E-4</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="K14">
+        <v>26</v>
+      </c>
+      <c r="N14">
         <f t="shared" si="8"/>
         <v>2.4787521766663585E-3</v>
       </c>
-      <c r="L14">
+      <c r="O14">
         <f t="shared" si="9"/>
         <v>-52.115337828390224</v>
       </c>

</xml_diff>

<commit_message>
updated schematic to match
</commit_message>
<xml_diff>
--- a/amp/amp.xlsx
+++ b/amp/amp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjk/projects/synthesizer/amp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3816991A-8C8B-2740-A148-4E200631E7EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08024AAD-4FE8-A746-AEBC-7007C9ABFBC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="28040" windowHeight="17540" xr2:uid="{6400FE91-138F-4D41-B9CE-9D9E08F46C3F}"/>
+    <workbookView xWindow="23200" yWindow="2800" windowWidth="28040" windowHeight="17540" xr2:uid="{6400FE91-138F-4D41-B9CE-9D9E08F46C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>VB/26mV</t>
   </si>
@@ -41,18 +41,12 @@
     <t>IC gain</t>
   </si>
   <si>
-    <t>gain</t>
-  </si>
-  <si>
     <t xml:space="preserve">DB gain </t>
   </si>
   <si>
     <t>cv-gain</t>
   </si>
   <si>
-    <t>resistor for V (kohm)</t>
-  </si>
-  <si>
     <t>IC (mA)</t>
   </si>
   <si>
@@ -78,6 +72,15 @@
   </si>
   <si>
     <t>Rref (kohm)</t>
+  </si>
+  <si>
+    <t>DB/V</t>
+  </si>
+  <si>
+    <t>Rout (kohm)</t>
+  </si>
+  <si>
+    <t>voltage gain</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541F8547-BF2A-374F-80CA-51B3B3BC1C08}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,12 +452,12 @@
     <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,46 +465,49 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-6</v>
       </c>
@@ -524,7 +530,7 @@
         <v>24</v>
       </c>
       <c r="G2">
-        <f>A2*0.026</f>
+        <f t="shared" ref="G2:G14" si="0">A2*0.026</f>
         <v>-0.156</v>
       </c>
       <c r="H2">
@@ -559,12 +565,12 @@
         <v>12.041199826559248</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-5</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B14" si="0">EXP(-1*A3)</f>
+        <f t="shared" ref="B3:B14" si="1">EXP(-1*A3)</f>
         <v>148.4131591025766</v>
       </c>
       <c r="C3">
@@ -574,685 +580,713 @@
         <v>0.5</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E14" si="1">MIN(C3,B3*D3)</f>
+        <f t="shared" ref="E3:E14" si="2">MIN(C3,B3*D3)</f>
         <v>2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F14" si="2">12/D3</f>
+        <f t="shared" ref="F3:F14" si="3">12/D3</f>
         <v>24</v>
       </c>
       <c r="G3">
-        <f>A3*0.026</f>
+        <f t="shared" si="0"/>
         <v>-0.13</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H14" si="3">-(3.3/120)</f>
+        <f t="shared" ref="H3:H14" si="4">-(3.3/120)</f>
         <v>-2.75E-2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I14" si="4">G3/H3</f>
+        <f t="shared" ref="I3:I14" si="5">G3/H3</f>
         <v>4.7272727272727275</v>
       </c>
       <c r="J3">
         <v>5</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K14" si="5">I3+J3</f>
+        <f t="shared" ref="K3:K14" si="6">I3+J3</f>
         <v>9.7272727272727266</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L14" si="6">0.5*(20/26)*E3</f>
+        <f t="shared" ref="L3:L14" si="7">0.5*(20/26)*E3</f>
         <v>0.76923076923076927</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M14" si="7">5/L$8</f>
+        <f t="shared" ref="M3:M14" si="8">5/L$8</f>
         <v>26</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N14" si="8">(L3*M3)/5</f>
+        <f t="shared" ref="N3:N14" si="9">(L3*M3)/5</f>
         <v>4</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O14" si="9">20*LOG10(N3)</f>
+        <f t="shared" ref="O3:O14" si="10">20*LOG10(N3)</f>
         <v>12.041199826559248</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-4</v>
       </c>
       <c r="B4">
+        <f t="shared" si="1"/>
+        <v>54.598150033144236</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="0"/>
-        <v>54.598150033144236</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="G4">
-        <f>A4*0.026</f>
         <v>-0.104</v>
       </c>
       <c r="H4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.75E-2</v>
       </c>
       <c r="I4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.7818181818181817</v>
       </c>
       <c r="J4">
         <v>5</v>
       </c>
       <c r="K4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.7818181818181813</v>
       </c>
       <c r="L4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="M4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="N4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="O4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.041199826559248</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-3</v>
       </c>
       <c r="B5">
+        <f t="shared" si="1"/>
+        <v>20.085536923187668</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="0"/>
-        <v>20.085536923187668</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>0.5</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="G5">
-        <f>A5*0.026</f>
         <v>-7.8E-2</v>
       </c>
       <c r="H5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.75E-2</v>
       </c>
       <c r="I5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.8363636363636364</v>
       </c>
       <c r="J5">
         <v>5</v>
       </c>
       <c r="K5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.836363636363636</v>
       </c>
       <c r="L5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="M5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="N5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="O5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.041199826559248</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-2</v>
       </c>
       <c r="B6">
+        <f t="shared" si="1"/>
+        <v>7.3890560989306504</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
-        <v>7.3890560989306504</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>0.5</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="G6">
-        <f>A6*0.026</f>
         <v>-5.1999999999999998E-2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.75E-2</v>
       </c>
       <c r="I6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.8909090909090909</v>
       </c>
       <c r="J6">
         <v>5</v>
       </c>
       <c r="K6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.8909090909090907</v>
       </c>
       <c r="L6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="M6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="N6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="O6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.041199826559248</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-1</v>
       </c>
       <c r="B7">
+        <f t="shared" si="1"/>
+        <v>2.7182818284590451</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>1.3591409142295225</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>2.7182818284590451</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>0.5</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
-        <v>1.3591409142295225</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="G7">
-        <f>A7*0.026</f>
         <v>-2.5999999999999999E-2</v>
       </c>
       <c r="H7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.75E-2</v>
       </c>
       <c r="I7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.94545454545454544</v>
       </c>
       <c r="J7">
         <v>5</v>
       </c>
       <c r="K7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.9454545454545453</v>
       </c>
       <c r="L7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.52274650547289336</v>
       </c>
       <c r="M7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="N7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.7182818284590455</v>
       </c>
       <c r="O7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.6858896380650368</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7">
+        <f>O7/I7</f>
+        <v>9.1869986556457128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="B8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>-2.75E-2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="7"/>
+        <v>0.19230769230769232</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>0.5</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="G8">
-        <f>A8*0.026</f>
+      <c r="O8">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="3"/>
-        <v>-2.75E-2</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="6"/>
-        <v>0.19230769230769232</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="7"/>
-        <v>26</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
+        <f t="shared" si="1"/>
+        <v>0.36787944117144233</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>0.18393972058572117</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
-        <v>0.36787944117144233</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
-        <v>0.5</v>
-      </c>
-      <c r="E9">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>-2.75E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>-0.94545454545454544</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="6"/>
+        <v>4.0545454545454547</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="7"/>
+        <v>7.0746046379123531E-2</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="9"/>
+        <v>0.36787944117144239</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="10"/>
+        <v>-8.685889638065035</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P8:P14" si="11">O9/I9</f>
+        <v>9.1869986556457111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
         <f t="shared" si="1"/>
-        <v>0.18393972058572117</v>
-      </c>
-      <c r="F9">
+        <v>0.1353352832366127</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="2"/>
+        <v>6.7667641618306351E-2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="G9">
-        <f>A9*0.026</f>
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="3"/>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="4"/>
-        <v>-0.94545454545454544</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9">
+      <c r="I10">
         <f t="shared" si="5"/>
-        <v>4.0545454545454547</v>
-      </c>
-      <c r="L9">
+        <v>-1.8909090909090909</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="6"/>
-        <v>7.0746046379123531E-2</v>
-      </c>
-      <c r="M9">
+        <v>3.1090909090909093</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="7"/>
+        <v>2.6026016007040905E-2</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
-      <c r="N9">
-        <f t="shared" si="8"/>
-        <v>0.36787944117144239</v>
-      </c>
-      <c r="O9">
+      <c r="N10">
         <f t="shared" si="9"/>
-        <v>-8.685889638065035</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
         <v>0.1353352832366127</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>0.5</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>6.7667641618306351E-2</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="G10">
-        <f>A10*0.026</f>
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="3"/>
-        <v>-2.75E-2</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="4"/>
-        <v>-1.8909090909090909</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="5"/>
-        <v>3.1090909090909093</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="6"/>
-        <v>2.6026016007040905E-2</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="7"/>
-        <v>26</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="8"/>
-        <v>0.1353352832366127</v>
-      </c>
       <c r="O10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-17.371779276130074</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10">
+        <f t="shared" si="11"/>
+        <v>9.1869986556457128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11">
+        <f t="shared" si="1"/>
+        <v>4.9787068367863944E-2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>2.4893534183931972E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
-        <v>4.9787068367863944E-2</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>0.5</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>2.4893534183931972E-2</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="G11">
-        <f>A11*0.026</f>
         <v>7.8E-2</v>
       </c>
       <c r="H11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-2.75E-2</v>
       </c>
       <c r="I11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2.8363636363636364</v>
       </c>
       <c r="J11">
         <v>5</v>
       </c>
       <c r="K11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.1636363636363636</v>
       </c>
       <c r="L11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.5744362245892209E-3</v>
       </c>
       <c r="M11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="N11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.9787068367863951E-2</v>
       </c>
       <c r="O11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-26.057668914195105</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11">
+        <f t="shared" si="11"/>
+        <v>9.1869986556457093</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12">
+        <f t="shared" si="1"/>
+        <v>1.8315638888734179E-2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>9.1578194443670893E-3</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
+        <v>0.104</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>-2.75E-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>-3.7818181818181817</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="6"/>
+        <v>1.2181818181818183</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="7"/>
+        <v>3.5222382478334959E-3</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="9"/>
         <v>1.8315638888734179E-2</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>0.5</v>
-      </c>
-      <c r="E12">
+      <c r="O12">
+        <f t="shared" si="10"/>
+        <v>-34.743558552260147</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="11"/>
+        <v>9.1869986556457128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
         <f t="shared" si="1"/>
-        <v>9.1578194443670893E-3</v>
-      </c>
-      <c r="F12">
+        <v>6.737946999085467E-3</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="2"/>
+        <v>3.3689734995427335E-3</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="G12">
-        <f>A12*0.026</f>
-        <v>0.104</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="3"/>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>0.13</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
         <v>-2.75E-2</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="4"/>
-        <v>-3.7818181818181817</v>
-      </c>
-      <c r="J12">
-        <v>5</v>
-      </c>
-      <c r="K12">
+      <c r="I13">
         <f t="shared" si="5"/>
-        <v>1.2181818181818183</v>
-      </c>
-      <c r="L12">
+        <v>-4.7272727272727275</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="6"/>
-        <v>3.5222382478334959E-3</v>
-      </c>
-      <c r="M12">
+        <v>0.27272727272727249</v>
+      </c>
+      <c r="L13">
         <f t="shared" si="7"/>
+        <v>1.2957590382856668E-3</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="8"/>
-        <v>1.8315638888734179E-2</v>
-      </c>
-      <c r="O12">
+      <c r="N13">
         <f t="shared" si="9"/>
-        <v>-34.743558552260147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
         <v>6.737946999085467E-3</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>0.5</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="1"/>
-        <v>3.3689734995427335E-3</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="G13">
-        <f>A13*0.026</f>
-        <v>0.13</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="3"/>
-        <v>-2.75E-2</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="4"/>
-        <v>-4.7272727272727275</v>
-      </c>
-      <c r="J13">
-        <v>5</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="5"/>
-        <v>0.27272727272727249</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="6"/>
-        <v>1.2957590382856668E-3</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="7"/>
-        <v>26</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="8"/>
-        <v>6.737946999085467E-3</v>
-      </c>
       <c r="O13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-43.429448190325182</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13">
+        <f t="shared" si="11"/>
+        <v>9.1869986556457111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14">
+        <f t="shared" si="1"/>
+        <v>2.4787521766663585E-3</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>1.2393760883331792E-3</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="0"/>
+        <v>0.156</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>-2.75E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>-5.6727272727272728</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="6"/>
+        <v>-0.67272727272727284</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="7"/>
+        <v>4.7668311089737667E-4</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="9"/>
         <v>2.4787521766663585E-3</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>0.5</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>1.2393760883331792E-3</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="G14">
-        <f>A14*0.026</f>
-        <v>0.156</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="3"/>
-        <v>-2.75E-2</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="4"/>
-        <v>-5.6727272727272728</v>
-      </c>
-      <c r="J14">
-        <v>5</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="5"/>
-        <v>-0.67272727272727284</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="6"/>
-        <v>4.7668311089737667E-4</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="7"/>
-        <v>26</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="8"/>
-        <v>2.4787521766663585E-3</v>
-      </c>
       <c r="O14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-52.115337828390224</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="11"/>
+        <v>9.1869986556457128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>